<commit_message>
add finalproject part 1
</commit_message>
<xml_diff>
--- a/TugasMingguKe-12/NNSklearn.xlsx
+++ b/TugasMingguKe-12/NNSklearn.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samsudhuha/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VIERI FATH\Documents\GitHub\TugasKK_B_Kelompok2\TugasMingguKe-12\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{36517B18-3702-924F-AE3E-CDE3B00A0423}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EB67EEF-8704-49B3-AB00-B5687AFF6D8A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{C10A229F-D972-D74A-BABB-A91CD0D6076F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{C10A229F-D972-D74A-BABB-A91CD0D6076F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="18">
   <si>
     <t>Model 1</t>
   </si>
@@ -70,6 +70,15 @@
   </si>
   <si>
     <t>0.005</t>
+  </si>
+  <si>
+    <t>logistic, tanha</t>
+  </si>
+  <si>
+    <t>sgd</t>
+  </si>
+  <si>
+    <t>lbfgs</t>
   </si>
 </sst>
 </file>
@@ -114,18 +123,18 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -442,457 +451,472 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEB2368E-74C1-AD4A-A177-021C7E5C6B5A}">
-  <dimension ref="A1:L16"/>
+  <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="10.83203125" style="3"/>
+    <col min="1" max="16384" width="10.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B2" s="3" t="s">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="3" t="s">
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="2">
         <v>0.9</v>
       </c>
-      <c r="J3" s="3">
+      <c r="J3" s="1">
         <v>0.89</v>
       </c>
-      <c r="K3" s="3">
+      <c r="K3" s="1">
         <v>0.9</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="3" t="s">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="2">
         <v>0.7</v>
       </c>
-      <c r="J4" s="3">
+      <c r="J4" s="1">
         <v>0.88</v>
       </c>
-      <c r="K4" s="3">
+      <c r="K4" s="1">
         <v>0.88</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" s="3" t="s">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="2">
         <v>0.5</v>
       </c>
-      <c r="J5" s="3">
+      <c r="J5" s="1">
         <v>0.89</v>
       </c>
-      <c r="K5" s="3">
+      <c r="K5" s="1">
         <v>0.89</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B6" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" s="3" t="s">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="2">
         <v>0.3</v>
       </c>
-      <c r="J6" s="3">
+      <c r="J6" s="1">
         <v>0.9</v>
       </c>
-      <c r="K6" s="3">
+      <c r="K6" s="1">
         <v>0.9</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B7" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" s="5" t="s">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="2">
         <v>0.9</v>
       </c>
-      <c r="J7" s="3">
+      <c r="J7" s="1">
         <v>0.85</v>
       </c>
-      <c r="K7" s="3">
+      <c r="K7" s="1">
         <v>0.84</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B8" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" s="5" t="s">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="2">
         <v>0.7</v>
       </c>
-      <c r="J8" s="3">
+      <c r="J8" s="1">
         <v>0.85</v>
       </c>
-      <c r="K8" s="3">
+      <c r="K8" s="1">
         <v>0.85</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B9" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H9" s="5" t="s">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I9" s="4">
+      <c r="I9" s="2">
         <v>0.5</v>
       </c>
-      <c r="J9" s="3">
+      <c r="J9" s="1">
         <v>0.89</v>
       </c>
-      <c r="K9" s="3">
+      <c r="K9" s="1">
         <v>0.89</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B10" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H10" s="5" t="s">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I10" s="4">
+      <c r="I10" s="2">
         <v>0.3</v>
       </c>
-      <c r="J10" s="3">
+      <c r="J10" s="1">
         <v>0.87</v>
       </c>
-      <c r="K10" s="3">
+      <c r="K10" s="1">
         <v>0.87</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B11" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H11" s="3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" s="1">
         <v>0.1</v>
       </c>
-      <c r="I11" s="4">
+      <c r="I11" s="2">
         <v>0.9</v>
       </c>
-      <c r="J11" s="3">
+      <c r="J11" s="1">
         <v>0.5</v>
       </c>
-      <c r="K11" s="3">
+      <c r="K11" s="1">
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B12" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H12" s="3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" s="1">
         <v>0.1</v>
       </c>
-      <c r="I12" s="4">
+      <c r="I12" s="2">
         <v>0.7</v>
       </c>
-      <c r="J12" s="3">
+      <c r="J12" s="1">
         <v>0.5</v>
       </c>
-      <c r="K12" s="3">
+      <c r="K12" s="1">
         <v>0.5</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B13" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H13" s="3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H13" s="1">
         <v>0.1</v>
       </c>
-      <c r="I13" s="4">
+      <c r="I13" s="2">
         <v>0.5</v>
       </c>
-      <c r="J13" s="3">
+      <c r="J13" s="1">
         <v>0.51</v>
       </c>
-      <c r="K13" s="3">
+      <c r="K13" s="1">
         <v>0.51</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B14" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H14" s="3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H14" s="1">
         <v>0.1</v>
       </c>
-      <c r="I14" s="4">
+      <c r="I14" s="2">
         <v>0.3</v>
       </c>
-      <c r="J14" s="3">
+      <c r="J14" s="1">
         <v>0.5</v>
       </c>
-      <c r="K14" s="3">
+      <c r="K14" s="1">
         <v>0.5</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="H16" s="5"/>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="H16" s="3"/>
+    </row>
+    <row r="18" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H18" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H19" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H20" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>